<commit_message>
customer registration test committed
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{14A3DC0A-B3B3-4DB7-A44D-31E749A4DBB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E40BE1CB-94D6-41F4-9180-4941C849D6B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="15405" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="15495" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -21,19 +21,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>vinaydev1982@gmail.com</t>
-  </si>
-  <si>
-    <t>Abcd@9876</t>
+    <t>admin@itwinetech.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,6 +40,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -71,8 +75,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -368,18 +373,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" s="1">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{2C40CE4C-6469-48B0-B8A9-8F6B2EFBF11E}"/>
-    <hyperlink ref="B1" r:id="rId2" xr:uid="{850B7076-0116-4EE4-9D3B-9A1894CCB5D0}"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{94314CBB-3BC3-418B-A7D1-21E0ADFCAD70}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>